<commit_message>
We have updated several pieces of the codebase for this submission to CCR. Specifically, we removed PD1-2 and AC-V32 for logistical reasons. I corrected a bug which the tumoronly filters were not properly indexing for printing of the filter fail status (but the good outputs were fine).
</commit_message>
<xml_diff>
--- a/tables/ASCC-supplementary_table1-somatic_mutations.xlsx
+++ b/tables/ASCC-supplementary_table1-somatic_mutations.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="15580" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="15580" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pilot Cohort" sheetId="1" r:id="rId1"/>
     <sheet name="Extension Cohort" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Extension Cohort'!$A$2:$T$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Extension Cohort'!$A$2:$T$73</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1321" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="308">
   <si>
     <t>Patient ID</t>
   </si>
@@ -508,451 +508,445 @@
     <t>c.3556C&gt;T</t>
   </si>
   <si>
+    <t>c.3140A&gt;G</t>
+  </si>
+  <si>
+    <t>c.742C&gt;T</t>
+  </si>
+  <si>
+    <t>c.45G&gt;A</t>
+  </si>
+  <si>
+    <t>c.817C&gt;T</t>
+  </si>
+  <si>
+    <t>c.844C&gt;T</t>
+  </si>
+  <si>
+    <t>c.1009C&gt;T</t>
+  </si>
+  <si>
+    <t>c.19C&gt;T</t>
+  </si>
+  <si>
+    <t>p.R1324K</t>
+  </si>
+  <si>
+    <t>p.Q3793*</t>
+  </si>
+  <si>
+    <t>p.W315*</t>
+  </si>
+  <si>
+    <t>p.V344G</t>
+  </si>
+  <si>
+    <t>p.Y1495*</t>
+  </si>
+  <si>
+    <t>p.A1713V</t>
+  </si>
+  <si>
+    <t>p.R2036H</t>
+  </si>
+  <si>
+    <t>p.S220F</t>
+  </si>
+  <si>
+    <t>p.S565R</t>
+  </si>
+  <si>
+    <t>p.P85S</t>
+  </si>
+  <si>
+    <t>p.H179L</t>
+  </si>
+  <si>
+    <t>p.R135K</t>
+  </si>
+  <si>
+    <t>p.E2536A</t>
+  </si>
+  <si>
+    <t>p.E2871K</t>
+  </si>
+  <si>
+    <t>p.G3500*</t>
+  </si>
+  <si>
+    <t>p.S462Y</t>
+  </si>
+  <si>
+    <t>p.G557E</t>
+  </si>
+  <si>
+    <t>p.L3136V</t>
+  </si>
+  <si>
+    <t>p.I436N</t>
+  </si>
+  <si>
+    <t>p.Q793*</t>
+  </si>
+  <si>
+    <t>p.Q482*</t>
+  </si>
+  <si>
+    <t>p.L249V</t>
+  </si>
+  <si>
+    <t>p.E1252*</t>
+  </si>
+  <si>
+    <t>p.R80Q</t>
+  </si>
+  <si>
+    <t>p.E180K</t>
+  </si>
+  <si>
+    <t>p.K2961N</t>
+  </si>
+  <si>
+    <t>p.S3373*</t>
+  </si>
+  <si>
+    <t>p.M270I</t>
+  </si>
+  <si>
+    <t>p.K188T</t>
+  </si>
+  <si>
+    <t>p.E552*</t>
+  </si>
+  <si>
+    <t>p.P3622S</t>
+  </si>
+  <si>
+    <t>p.S3638*</t>
+  </si>
+  <si>
+    <t>p.Q214*</t>
+  </si>
+  <si>
+    <t>p.C327F</t>
+  </si>
+  <si>
+    <t>p.Q417R</t>
+  </si>
+  <si>
+    <t>p.Q1186*</t>
+  </si>
+  <si>
+    <t>p.H1047R</t>
+  </si>
+  <si>
+    <t>p.R248W</t>
+  </si>
+  <si>
+    <t>p.W15*</t>
+  </si>
+  <si>
+    <t>p.R273C</t>
+  </si>
+  <si>
+    <t>p.R282W</t>
+  </si>
+  <si>
+    <t>p.R337C</t>
+  </si>
+  <si>
+    <t>p.R7*</t>
+  </si>
+  <si>
+    <t>AC-P02</t>
+  </si>
+  <si>
+    <t>AC-P04</t>
+  </si>
+  <si>
+    <t>AC-P06</t>
+  </si>
+  <si>
+    <t>AC-P07</t>
+  </si>
+  <si>
+    <t>AC-P08</t>
+  </si>
+  <si>
+    <t>AC-P09</t>
+  </si>
+  <si>
+    <t>AC-P10</t>
+  </si>
+  <si>
+    <t>AC-P11</t>
+  </si>
+  <si>
+    <t>AC-P12</t>
+  </si>
+  <si>
+    <t>AC-P14</t>
+  </si>
+  <si>
+    <t>AC-P15</t>
+  </si>
+  <si>
+    <t>AC_PD1</t>
+  </si>
+  <si>
+    <t>AC-V01</t>
+  </si>
+  <si>
+    <t>AC-V03</t>
+  </si>
+  <si>
+    <t>AC-V04</t>
+  </si>
+  <si>
+    <t>AC-V05</t>
+  </si>
+  <si>
+    <t>AC-V06</t>
+  </si>
+  <si>
+    <t>AC-V07</t>
+  </si>
+  <si>
+    <t>AC-V08</t>
+  </si>
+  <si>
+    <t>AC-V09</t>
+  </si>
+  <si>
+    <t>AC-V10</t>
+  </si>
+  <si>
+    <t>AC-V11</t>
+  </si>
+  <si>
+    <t>AC-V12</t>
+  </si>
+  <si>
+    <t>AC-V14</t>
+  </si>
+  <si>
+    <t>AC-V15</t>
+  </si>
+  <si>
+    <t>AC-V16</t>
+  </si>
+  <si>
+    <t>AC-V17</t>
+  </si>
+  <si>
+    <t>AC-V18</t>
+  </si>
+  <si>
+    <t>AC-V21</t>
+  </si>
+  <si>
+    <t>AC-V23</t>
+  </si>
+  <si>
+    <t>AC-V25</t>
+  </si>
+  <si>
+    <t>AC-V26</t>
+  </si>
+  <si>
+    <t>AC-V28</t>
+  </si>
+  <si>
+    <t>AC-V29</t>
+  </si>
+  <si>
+    <t>AC-V30</t>
+  </si>
+  <si>
+    <t>AC-V31</t>
+  </si>
+  <si>
+    <t># Supplementary Table 1.1: Somatic mutations and short insertion / deletions, Pilot Cohort, ASCC gene list</t>
+  </si>
+  <si>
+    <t># Supplementary Table 1.2: Somatic mutations and short insertion / deletions, Extension Cohort, ASCC gene list</t>
+  </si>
+  <si>
+    <t>AC-DFCI_AC_PD1-1-Tumor-SM-9LRI9</t>
+  </si>
+  <si>
+    <t>AC-P02-Tumor-SM-63B4K</t>
+  </si>
+  <si>
+    <t>AC-P04-Tumor-SM-63B4Q</t>
+  </si>
+  <si>
+    <t>AC-P06-Tumor-SM-63B4T</t>
+  </si>
+  <si>
+    <t>AC-P07-Tumor-SM-63B4V</t>
+  </si>
+  <si>
+    <t>AC-P08-Tumor-SM-63B4X</t>
+  </si>
+  <si>
+    <t>AC-P09-Tumor-SM-63B4Z</t>
+  </si>
+  <si>
+    <t>AC-P09-Tumor-SM-63B52</t>
+  </si>
+  <si>
+    <t>AC-P10-Tumor-SM-63B53</t>
+  </si>
+  <si>
+    <t>AC-P11-Tumor-SM-63B56</t>
+  </si>
+  <si>
+    <t>AC-P12-Tumor-SM-63B58</t>
+  </si>
+  <si>
+    <t>AC-P12-Tumor-SM-63B59</t>
+  </si>
+  <si>
+    <t>AC-P14-Tumor-SM-63B5C</t>
+  </si>
+  <si>
+    <t>AC-P15-Tumor-SM-63B5D</t>
+  </si>
+  <si>
+    <t>AC-P15-Tumor-SM-63B5F</t>
+  </si>
+  <si>
+    <t>No Response</t>
+  </si>
+  <si>
+    <t>Clinical Outcome</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>Sample ID</t>
+  </si>
+  <si>
+    <t>AC-V01-Tumor-SM-9J45S</t>
+  </si>
+  <si>
+    <t>AC-V03-Tumor-SM-9J45U</t>
+  </si>
+  <si>
+    <t>AC-V04-Tumor-SM-9J45V</t>
+  </si>
+  <si>
+    <t>AC-V05-Tumor-SM-9J45W</t>
+  </si>
+  <si>
+    <t>AC-V06-Tumor-SM-9J45X</t>
+  </si>
+  <si>
+    <t>AC-V07-Tumor-SM-9J45Y</t>
+  </si>
+  <si>
+    <t>AC-V08-Tumor-SM-9J45Z</t>
+  </si>
+  <si>
+    <t>AC-V08-Tumor-SM-9J461</t>
+  </si>
+  <si>
+    <t>AC-V08-Tumor-SM-9J462</t>
+  </si>
+  <si>
+    <t>AC-V09-Tumor-SM-9J463</t>
+  </si>
+  <si>
+    <t>AC-V09-Tumor-SM-9J464</t>
+  </si>
+  <si>
+    <t>AC-V10-Tumor-SM-9J465</t>
+  </si>
+  <si>
+    <t>AC-V10-Tumor-SM-9J466</t>
+  </si>
+  <si>
+    <t>AC-V11-Tumor-SM-9J467</t>
+  </si>
+  <si>
+    <t>AC-V11-Tumor-SM-9J468</t>
+  </si>
+  <si>
+    <t>AC-V12-Tumor-SM-9J46A</t>
+  </si>
+  <si>
+    <t>AC-V12-Tumor-SM-9N4BH</t>
+  </si>
+  <si>
+    <t>AC-V14-Tumor-SM-9J46C</t>
+  </si>
+  <si>
+    <t>AC-V14-Tumor-SM-9J46D</t>
+  </si>
+  <si>
+    <t>AC-V15-Tumor-SM-9J46E</t>
+  </si>
+  <si>
+    <t>AC-V15-Tumor-SM-9J46F</t>
+  </si>
+  <si>
+    <t>AC-V16-Tumor-SM-9J46G</t>
+  </si>
+  <si>
+    <t>AC-V16-Tumor-SM-9J46H</t>
+  </si>
+  <si>
+    <t>AC-V17-Tumor-SM-9J46I</t>
+  </si>
+  <si>
+    <t>AC-V18-Tumor-SM-9J46J</t>
+  </si>
+  <si>
+    <t>AC-V18-Tumor-SM-9J46K</t>
+  </si>
+  <si>
+    <t>AC-V21-Tumor-SM-9J46N</t>
+  </si>
+  <si>
+    <t>AC-V23-Tumor-SM-9J46P</t>
+  </si>
+  <si>
+    <t>AC-V25-Tumor-SM-9J46R</t>
+  </si>
+  <si>
+    <t>AC-V26-Tumor-SM-9J46S</t>
+  </si>
+  <si>
+    <t>AC-V28-Tumor-SM-9J46U</t>
+  </si>
+  <si>
+    <t>AC-V29-Tumor-SM-9J46V</t>
+  </si>
+  <si>
+    <t>AC-V30-Tumor-SM-9J46W</t>
+  </si>
+  <si>
+    <t>AC-V31-Tumor-SM-9J46X</t>
+  </si>
+  <si>
+    <t>AC-V34</t>
+  </si>
+  <si>
+    <t>AC-V34-Tumor-SM-9J471</t>
+  </si>
+  <si>
     <t>c.1678G&gt;C</t>
   </si>
   <si>
+    <t>p.D560H</t>
+  </si>
+  <si>
     <t>c.1673C&gt;T</t>
   </si>
   <si>
-    <t>c.3140A&gt;G</t>
-  </si>
-  <si>
-    <t>c.742C&gt;T</t>
-  </si>
-  <si>
-    <t>c.45G&gt;A</t>
-  </si>
-  <si>
-    <t>c.817C&gt;T</t>
-  </si>
-  <si>
-    <t>c.844C&gt;T</t>
-  </si>
-  <si>
-    <t>c.1009C&gt;T</t>
-  </si>
-  <si>
-    <t>c.19C&gt;T</t>
-  </si>
-  <si>
-    <t>p.R1324K</t>
-  </si>
-  <si>
-    <t>p.Q3793*</t>
-  </si>
-  <si>
-    <t>p.W315*</t>
-  </si>
-  <si>
-    <t>p.V344G</t>
-  </si>
-  <si>
-    <t>p.Y1495*</t>
-  </si>
-  <si>
-    <t>p.A1713V</t>
-  </si>
-  <si>
-    <t>p.R2036H</t>
-  </si>
-  <si>
-    <t>p.S220F</t>
-  </si>
-  <si>
-    <t>p.S565R</t>
-  </si>
-  <si>
-    <t>p.P85S</t>
-  </si>
-  <si>
-    <t>p.H179L</t>
-  </si>
-  <si>
-    <t>p.R135K</t>
-  </si>
-  <si>
-    <t>p.E2536A</t>
-  </si>
-  <si>
-    <t>p.E2871K</t>
-  </si>
-  <si>
-    <t>p.G3500*</t>
-  </si>
-  <si>
-    <t>p.S462Y</t>
-  </si>
-  <si>
-    <t>p.G557E</t>
-  </si>
-  <si>
-    <t>p.L3136V</t>
-  </si>
-  <si>
-    <t>p.I436N</t>
-  </si>
-  <si>
-    <t>p.Q793*</t>
-  </si>
-  <si>
-    <t>p.Q482*</t>
-  </si>
-  <si>
-    <t>p.L249V</t>
-  </si>
-  <si>
-    <t>p.E1252*</t>
-  </si>
-  <si>
-    <t>p.R80Q</t>
-  </si>
-  <si>
-    <t>p.E180K</t>
-  </si>
-  <si>
-    <t>p.K2961N</t>
-  </si>
-  <si>
-    <t>p.S3373*</t>
-  </si>
-  <si>
-    <t>p.M270I</t>
-  </si>
-  <si>
-    <t>p.K188T</t>
-  </si>
-  <si>
-    <t>p.E552*</t>
-  </si>
-  <si>
-    <t>p.P3622S</t>
-  </si>
-  <si>
-    <t>p.S3638*</t>
-  </si>
-  <si>
-    <t>p.Q214*</t>
-  </si>
-  <si>
-    <t>p.C327F</t>
-  </si>
-  <si>
-    <t>p.Q417R</t>
-  </si>
-  <si>
-    <t>p.Q1186*</t>
-  </si>
-  <si>
-    <t>p.D560H</t>
-  </si>
-  <si>
     <t>p.S558F</t>
-  </si>
-  <si>
-    <t>p.H1047R</t>
-  </si>
-  <si>
-    <t>p.R248W</t>
-  </si>
-  <si>
-    <t>p.W15*</t>
-  </si>
-  <si>
-    <t>p.R273C</t>
-  </si>
-  <si>
-    <t>p.R282W</t>
-  </si>
-  <si>
-    <t>p.R337C</t>
-  </si>
-  <si>
-    <t>p.R7*</t>
-  </si>
-  <si>
-    <t>AC-P02</t>
-  </si>
-  <si>
-    <t>AC-P04</t>
-  </si>
-  <si>
-    <t>AC-P06</t>
-  </si>
-  <si>
-    <t>AC-P07</t>
-  </si>
-  <si>
-    <t>AC-P08</t>
-  </si>
-  <si>
-    <t>AC-P09</t>
-  </si>
-  <si>
-    <t>AC-P10</t>
-  </si>
-  <si>
-    <t>AC-P11</t>
-  </si>
-  <si>
-    <t>AC-P12</t>
-  </si>
-  <si>
-    <t>AC-P14</t>
-  </si>
-  <si>
-    <t>AC-P15</t>
-  </si>
-  <si>
-    <t>AC_PD1</t>
-  </si>
-  <si>
-    <t>AC-V01</t>
-  </si>
-  <si>
-    <t>AC-V03</t>
-  </si>
-  <si>
-    <t>AC-V04</t>
-  </si>
-  <si>
-    <t>AC-V05</t>
-  </si>
-  <si>
-    <t>AC-V06</t>
-  </si>
-  <si>
-    <t>AC-V07</t>
-  </si>
-  <si>
-    <t>AC-V08</t>
-  </si>
-  <si>
-    <t>AC-V09</t>
-  </si>
-  <si>
-    <t>AC-V10</t>
-  </si>
-  <si>
-    <t>AC-V11</t>
-  </si>
-  <si>
-    <t>AC-V12</t>
-  </si>
-  <si>
-    <t>AC-V14</t>
-  </si>
-  <si>
-    <t>AC-V15</t>
-  </si>
-  <si>
-    <t>AC-V16</t>
-  </si>
-  <si>
-    <t>AC-V17</t>
-  </si>
-  <si>
-    <t>AC-V18</t>
-  </si>
-  <si>
-    <t>AC-V21</t>
-  </si>
-  <si>
-    <t>AC-V23</t>
-  </si>
-  <si>
-    <t>AC-V25</t>
-  </si>
-  <si>
-    <t>AC-V26</t>
-  </si>
-  <si>
-    <t>AC-V28</t>
-  </si>
-  <si>
-    <t>AC-V29</t>
-  </si>
-  <si>
-    <t>AC-V30</t>
-  </si>
-  <si>
-    <t>AC-V31</t>
-  </si>
-  <si>
-    <t>AC-V32</t>
-  </si>
-  <si>
-    <t>AC-V34</t>
-  </si>
-  <si>
-    <t># Supplementary Table 1.1: Somatic mutations and short insertion / deletions, Pilot Cohort, ASCC gene list</t>
-  </si>
-  <si>
-    <t># Supplementary Table 1.2: Somatic mutations and short insertion / deletions, Extension Cohort, ASCC gene list</t>
-  </si>
-  <si>
-    <t>AC-DFCI_AC_PD1-1-Tumor-SM-9LRI9</t>
-  </si>
-  <si>
-    <t>AC-P02-Tumor-SM-63B4K</t>
-  </si>
-  <si>
-    <t>AC-P04-Tumor-SM-63B4Q</t>
-  </si>
-  <si>
-    <t>AC-P06-Tumor-SM-63B4T</t>
-  </si>
-  <si>
-    <t>AC-P07-Tumor-SM-63B4V</t>
-  </si>
-  <si>
-    <t>AC-P08-Tumor-SM-63B4X</t>
-  </si>
-  <si>
-    <t>AC-P09-Tumor-SM-63B4Z</t>
-  </si>
-  <si>
-    <t>AC-P09-Tumor-SM-63B52</t>
-  </si>
-  <si>
-    <t>AC-P10-Tumor-SM-63B53</t>
-  </si>
-  <si>
-    <t>AC-P11-Tumor-SM-63B56</t>
-  </si>
-  <si>
-    <t>AC-P12-Tumor-SM-63B58</t>
-  </si>
-  <si>
-    <t>AC-P12-Tumor-SM-63B59</t>
-  </si>
-  <si>
-    <t>AC-P14-Tumor-SM-63B5C</t>
-  </si>
-  <si>
-    <t>AC-P15-Tumor-SM-63B5D</t>
-  </si>
-  <si>
-    <t>AC-P15-Tumor-SM-63B5F</t>
-  </si>
-  <si>
-    <t>No Response</t>
-  </si>
-  <si>
-    <t>Clinical Outcome</t>
-  </si>
-  <si>
-    <t>Response</t>
-  </si>
-  <si>
-    <t>Sample ID</t>
-  </si>
-  <si>
-    <t>AC-V01-Tumor-SM-9J45S</t>
-  </si>
-  <si>
-    <t>AC-V03-Tumor-SM-9J45U</t>
-  </si>
-  <si>
-    <t>AC-V04-Tumor-SM-9J45V</t>
-  </si>
-  <si>
-    <t>AC-V05-Tumor-SM-9J45W</t>
-  </si>
-  <si>
-    <t>AC-V06-Tumor-SM-9J45X</t>
-  </si>
-  <si>
-    <t>AC-V07-Tumor-SM-9J45Y</t>
-  </si>
-  <si>
-    <t>AC-V08-Tumor-SM-9J45Z</t>
-  </si>
-  <si>
-    <t>AC-V08-Tumor-SM-9J461</t>
-  </si>
-  <si>
-    <t>AC-V08-Tumor-SM-9J462</t>
-  </si>
-  <si>
-    <t>AC-V09-Tumor-SM-9J463</t>
-  </si>
-  <si>
-    <t>AC-V09-Tumor-SM-9J464</t>
-  </si>
-  <si>
-    <t>AC-V10-Tumor-SM-9J465</t>
-  </si>
-  <si>
-    <t>AC-V10-Tumor-SM-9J466</t>
-  </si>
-  <si>
-    <t>AC-V11-Tumor-SM-9J467</t>
-  </si>
-  <si>
-    <t>AC-V11-Tumor-SM-9J468</t>
-  </si>
-  <si>
-    <t>AC-V12-Tumor-SM-9J46A</t>
-  </si>
-  <si>
-    <t>AC-V12-Tumor-SM-9N4BH</t>
-  </si>
-  <si>
-    <t>AC-V14-Tumor-SM-9J46C</t>
-  </si>
-  <si>
-    <t>AC-V14-Tumor-SM-9J46D</t>
-  </si>
-  <si>
-    <t>AC-V15-Tumor-SM-9J46E</t>
-  </si>
-  <si>
-    <t>AC-V15-Tumor-SM-9J46F</t>
-  </si>
-  <si>
-    <t>AC-V16-Tumor-SM-9J46G</t>
-  </si>
-  <si>
-    <t>AC-V16-Tumor-SM-9J46H</t>
-  </si>
-  <si>
-    <t>AC-V17-Tumor-SM-9J46I</t>
-  </si>
-  <si>
-    <t>AC-V18-Tumor-SM-9J46J</t>
-  </si>
-  <si>
-    <t>AC-V18-Tumor-SM-9J46K</t>
-  </si>
-  <si>
-    <t>AC-V21-Tumor-SM-9J46N</t>
-  </si>
-  <si>
-    <t>AC-V23-Tumor-SM-9J46P</t>
-  </si>
-  <si>
-    <t>AC-V25-Tumor-SM-9J46R</t>
-  </si>
-  <si>
-    <t>AC-V26-Tumor-SM-9J46S</t>
-  </si>
-  <si>
-    <t>AC-V28-Tumor-SM-9J46U</t>
-  </si>
-  <si>
-    <t>AC-V29-Tumor-SM-9J46V</t>
-  </si>
-  <si>
-    <t>AC-V30-Tumor-SM-9J46W</t>
-  </si>
-  <si>
-    <t>AC-V31-Tumor-SM-9J46X</t>
-  </si>
-  <si>
-    <t>AC-V32-Tumor-SM-9J46Y</t>
-  </si>
-  <si>
-    <t>AC-V34-Tumor-SM-9J471</t>
   </si>
 </sst>
 </file>
@@ -1471,8 +1465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1499,7 +1493,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -1507,10 +1501,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C2" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1563,13 +1557,13 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -1622,13 +1616,13 @@
     </row>
     <row r="4" spans="1:19">
       <c r="A4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C4" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
@@ -1681,13 +1675,13 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C5" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
@@ -1740,13 +1734,13 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C6" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
@@ -1799,13 +1793,13 @@
     </row>
     <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C7" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
@@ -1858,13 +1852,13 @@
     </row>
     <row r="8" spans="1:19">
       <c r="A8" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C8" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D8" t="s">
         <v>20</v>
@@ -1917,13 +1911,13 @@
     </row>
     <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C9" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
@@ -1976,13 +1970,13 @@
     </row>
     <row r="10" spans="1:19">
       <c r="A10" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C10" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D10" t="s">
         <v>23</v>
@@ -2035,13 +2029,13 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C11" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D11" t="s">
         <v>24</v>
@@ -2094,13 +2088,13 @@
     </row>
     <row r="12" spans="1:19">
       <c r="A12" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C12" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D12" t="s">
         <v>23</v>
@@ -2153,13 +2147,13 @@
     </row>
     <row r="13" spans="1:19">
       <c r="A13" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C13" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D13" t="s">
         <v>25</v>
@@ -2212,13 +2206,13 @@
     </row>
     <row r="14" spans="1:19">
       <c r="A14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C14" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D14" t="s">
         <v>26</v>
@@ -2271,13 +2265,13 @@
     </row>
     <row r="15" spans="1:19">
       <c r="A15" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C15" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D15" t="s">
         <v>27</v>
@@ -2330,13 +2324,13 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C16" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D16" t="s">
         <v>28</v>
@@ -2389,13 +2383,13 @@
     </row>
     <row r="17" spans="1:19">
       <c r="A17" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C17" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D17" t="s">
         <v>20</v>
@@ -2448,13 +2442,13 @@
     </row>
     <row r="18" spans="1:19">
       <c r="A18" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C18" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D18" t="s">
         <v>29</v>
@@ -2507,13 +2501,13 @@
     </row>
     <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C19" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D19" t="s">
         <v>30</v>
@@ -2566,13 +2560,13 @@
     </row>
     <row r="20" spans="1:19">
       <c r="A20" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C20" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D20" t="s">
         <v>30</v>
@@ -2625,13 +2619,13 @@
     </row>
     <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C21" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
@@ -2684,13 +2678,13 @@
     </row>
     <row r="22" spans="1:19">
       <c r="A22" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C22" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D22" t="s">
         <v>17</v>
@@ -2743,13 +2737,13 @@
     </row>
     <row r="23" spans="1:19">
       <c r="A23" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C23" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D23" t="s">
         <v>29</v>
@@ -2802,13 +2796,13 @@
     </row>
     <row r="24" spans="1:19">
       <c r="A24" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C24" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D24" t="s">
         <v>28</v>
@@ -2861,13 +2855,13 @@
     </row>
     <row r="25" spans="1:19">
       <c r="A25" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C25" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D25" t="s">
         <v>31</v>
@@ -2920,13 +2914,13 @@
     </row>
     <row r="26" spans="1:19">
       <c r="A26" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C26" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D26" t="s">
         <v>32</v>
@@ -2979,13 +2973,13 @@
     </row>
     <row r="27" spans="1:19">
       <c r="A27" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C27" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D27" t="s">
         <v>30</v>
@@ -3038,13 +3032,13 @@
     </row>
     <row r="28" spans="1:19">
       <c r="A28" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C28" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D28" t="s">
         <v>33</v>
@@ -3097,13 +3091,13 @@
     </row>
     <row r="29" spans="1:19">
       <c r="A29" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C29" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D29" t="s">
         <v>30</v>
@@ -3156,13 +3150,13 @@
     </row>
     <row r="30" spans="1:19">
       <c r="A30" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C30" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D30" t="s">
         <v>33</v>
@@ -3215,13 +3209,13 @@
     </row>
     <row r="31" spans="1:19">
       <c r="A31" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C31" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D31" t="s">
         <v>17</v>
@@ -3274,13 +3268,13 @@
     </row>
     <row r="32" spans="1:19">
       <c r="A32" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C32" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D32" t="s">
         <v>30</v>
@@ -3333,13 +3327,13 @@
     </row>
     <row r="33" spans="1:19">
       <c r="A33" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C33" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D33" t="s">
         <v>31</v>
@@ -3392,13 +3386,13 @@
     </row>
     <row r="34" spans="1:19">
       <c r="A34" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C34" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D34" t="s">
         <v>33</v>
@@ -3451,13 +3445,13 @@
     </row>
     <row r="35" spans="1:19">
       <c r="A35" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C35" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D35" t="s">
         <v>30</v>
@@ -3510,13 +3504,13 @@
     </row>
     <row r="36" spans="1:19">
       <c r="A36" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C36" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D36" t="s">
         <v>34</v>
@@ -3569,13 +3563,13 @@
     </row>
     <row r="37" spans="1:19">
       <c r="A37" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C37" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D37" t="s">
         <v>29</v>
@@ -3628,13 +3622,13 @@
     </row>
     <row r="38" spans="1:19">
       <c r="A38" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C38" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D38" t="s">
         <v>30</v>
@@ -3687,13 +3681,13 @@
     </row>
     <row r="39" spans="1:19">
       <c r="A39" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C39" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D39" t="s">
         <v>25</v>
@@ -3746,13 +3740,13 @@
     </row>
     <row r="40" spans="1:19">
       <c r="A40" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C40" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D40" t="s">
         <v>30</v>
@@ -3805,13 +3799,13 @@
     </row>
     <row r="41" spans="1:19">
       <c r="A41" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C41" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D41" t="s">
         <v>18</v>
@@ -3864,13 +3858,13 @@
     </row>
     <row r="42" spans="1:19">
       <c r="A42" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C42" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D42" t="s">
         <v>35</v>
@@ -3923,13 +3917,13 @@
     </row>
     <row r="43" spans="1:19">
       <c r="A43" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C43" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D43" t="s">
         <v>35</v>
@@ -3982,13 +3976,13 @@
     </row>
     <row r="44" spans="1:19">
       <c r="A44" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C44" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D44" t="s">
         <v>36</v>
@@ -4052,10 +4046,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S77"/>
+  <dimension ref="A1:S76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4084,7 +4078,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -4093,10 +4087,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C2" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -4149,13 +4143,13 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B3" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="C3" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
@@ -4194,7 +4188,7 @@
         <v>125</v>
       </c>
       <c r="P3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q3">
         <v>0.45923900000000001</v>
@@ -4208,13 +4202,13 @@
     </row>
     <row r="4" spans="1:19">
       <c r="A4" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B4" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -4250,10 +4244,10 @@
         <v>45</v>
       </c>
       <c r="O4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="P4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="Q4">
         <v>0.35102</v>
@@ -4267,13 +4261,13 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B5" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C5" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
@@ -4312,7 +4306,7 @@
         <v>126</v>
       </c>
       <c r="P5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="Q5">
         <v>0.38461499999999998</v>
@@ -4326,13 +4320,13 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B6" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C6" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -4385,13 +4379,13 @@
     </row>
     <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B7" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C7" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
@@ -4430,7 +4424,7 @@
         <v>127</v>
       </c>
       <c r="P7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="Q7">
         <v>0.102941</v>
@@ -4444,13 +4438,13 @@
     </row>
     <row r="8" spans="1:19">
       <c r="A8" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B8" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C8" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D8" t="s">
         <v>24</v>
@@ -4503,13 +4497,13 @@
     </row>
     <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B9" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C9" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D9" t="s">
         <v>17</v>
@@ -4548,7 +4542,7 @@
         <v>128</v>
       </c>
       <c r="P9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="Q9">
         <v>0.132075</v>
@@ -4562,13 +4556,13 @@
     </row>
     <row r="10" spans="1:19">
       <c r="A10" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B10" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C10" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -4621,13 +4615,13 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B11" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C11" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
@@ -4666,7 +4660,7 @@
         <v>129</v>
       </c>
       <c r="P11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="Q11">
         <v>0.23943700000000001</v>
@@ -4680,13 +4674,13 @@
     </row>
     <row r="12" spans="1:19">
       <c r="A12" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B12" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C12" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -4739,13 +4733,13 @@
     </row>
     <row r="13" spans="1:19">
       <c r="A13" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B13" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="C13" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D13" t="s">
         <v>25</v>
@@ -4784,7 +4778,7 @@
         <v>130</v>
       </c>
       <c r="P13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="Q13">
         <v>0.62616799999999995</v>
@@ -4798,13 +4792,13 @@
     </row>
     <row r="14" spans="1:19">
       <c r="A14" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B14" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="C14" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D14" t="s">
         <v>25</v>
@@ -4843,7 +4837,7 @@
         <v>130</v>
       </c>
       <c r="P14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="Q14">
         <v>0.65822800000000004</v>
@@ -4857,13 +4851,13 @@
     </row>
     <row r="15" spans="1:19">
       <c r="A15" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B15" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C15" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D15" t="s">
         <v>25</v>
@@ -4902,7 +4896,7 @@
         <v>130</v>
       </c>
       <c r="P15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="Q15">
         <v>0.63768100000000005</v>
@@ -4916,13 +4910,13 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B16" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C16" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D16" t="s">
         <v>25</v>
@@ -4961,7 +4955,7 @@
         <v>131</v>
       </c>
       <c r="P16" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="Q16">
         <v>0.17346900000000001</v>
@@ -4975,13 +4969,13 @@
     </row>
     <row r="17" spans="1:19">
       <c r="A17" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B17" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C17" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D17" t="s">
         <v>25</v>
@@ -5020,7 +5014,7 @@
         <v>131</v>
       </c>
       <c r="P17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="Q17">
         <v>0.40404000000000001</v>
@@ -5034,13 +5028,13 @@
     </row>
     <row r="18" spans="1:19">
       <c r="A18" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B18" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C18" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D18" t="s">
         <v>24</v>
@@ -5093,13 +5087,13 @@
     </row>
     <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B19" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="C19" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D19" t="s">
         <v>27</v>
@@ -5138,7 +5132,7 @@
         <v>132</v>
       </c>
       <c r="P19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Q19">
         <v>8.4336999999999995E-2</v>
@@ -5152,13 +5146,13 @@
     </row>
     <row r="20" spans="1:19">
       <c r="A20" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B20" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="C20" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D20" t="s">
         <v>120</v>
@@ -5197,7 +5191,7 @@
         <v>133</v>
       </c>
       <c r="P20" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Q20">
         <v>7.1038000000000004E-2</v>
@@ -5211,13 +5205,13 @@
     </row>
     <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B21" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="C21" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D21" t="s">
         <v>17</v>
@@ -5270,13 +5264,13 @@
     </row>
     <row r="22" spans="1:19">
       <c r="A22" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B22" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="C22" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D22" t="s">
         <v>17</v>
@@ -5329,13 +5323,13 @@
     </row>
     <row r="23" spans="1:19">
       <c r="A23" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B23" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C23" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D23" t="s">
         <v>120</v>
@@ -5374,7 +5368,7 @@
         <v>134</v>
       </c>
       <c r="P23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="Q23">
         <v>0.39181300000000002</v>
@@ -5388,13 +5382,13 @@
     </row>
     <row r="24" spans="1:19">
       <c r="A24" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B24" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="C24" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D24" t="s">
         <v>120</v>
@@ -5433,7 +5427,7 @@
         <v>134</v>
       </c>
       <c r="P24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="Q24">
         <v>0.138462</v>
@@ -5447,13 +5441,13 @@
     </row>
     <row r="25" spans="1:19">
       <c r="A25" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B25" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C25" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -5492,7 +5486,7 @@
         <v>135</v>
       </c>
       <c r="P25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="Q25">
         <v>0.2</v>
@@ -5506,13 +5500,13 @@
     </row>
     <row r="26" spans="1:19">
       <c r="A26" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B26" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C26" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D26" t="s">
         <v>34</v>
@@ -5551,7 +5545,7 @@
         <v>136</v>
       </c>
       <c r="P26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="Q26">
         <v>0.14583299999999999</v>
@@ -5565,13 +5559,13 @@
     </row>
     <row r="27" spans="1:19">
       <c r="A27" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B27" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C27" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D27" t="s">
         <v>28</v>
@@ -5607,10 +5601,10 @@
         <v>45</v>
       </c>
       <c r="O27" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="P27" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="Q27">
         <v>0.157303</v>
@@ -5624,13 +5618,13 @@
     </row>
     <row r="28" spans="1:19">
       <c r="A28" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B28" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C28" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D28" t="s">
         <v>122</v>
@@ -5666,10 +5660,10 @@
         <v>45</v>
       </c>
       <c r="O28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="P28" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="Q28">
         <v>0.31707299999999999</v>
@@ -5683,13 +5677,13 @@
     </row>
     <row r="29" spans="1:19">
       <c r="A29" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B29" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C29" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D29" t="s">
         <v>28</v>
@@ -5728,7 +5722,7 @@
         <v>135</v>
       </c>
       <c r="P29" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="Q29">
         <v>0.5</v>
@@ -5742,13 +5736,13 @@
     </row>
     <row r="30" spans="1:19">
       <c r="A30" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B30" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C30" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D30" t="s">
         <v>122</v>
@@ -5784,10 +5778,10 @@
         <v>45</v>
       </c>
       <c r="O30" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="P30" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="Q30">
         <v>0.24</v>
@@ -5801,13 +5795,13 @@
     </row>
     <row r="31" spans="1:19">
       <c r="A31" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B31" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="C31" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D31" t="s">
         <v>25</v>
@@ -5846,7 +5840,7 @@
         <v>137</v>
       </c>
       <c r="P31" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="Q31">
         <v>0.08</v>
@@ -5860,13 +5854,13 @@
     </row>
     <row r="32" spans="1:19">
       <c r="A32" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B32" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="C32" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D32" t="s">
         <v>17</v>
@@ -5919,13 +5913,13 @@
     </row>
     <row r="33" spans="1:19">
       <c r="A33" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B33" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="C33" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D33" t="s">
         <v>17</v>
@@ -5978,13 +5972,13 @@
     </row>
     <row r="34" spans="1:19">
       <c r="A34" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B34" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C34" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D34" t="s">
         <v>18</v>
@@ -6023,7 +6017,7 @@
         <v>138</v>
       </c>
       <c r="P34" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="Q34">
         <v>0.27027000000000001</v>
@@ -6037,13 +6031,13 @@
     </row>
     <row r="35" spans="1:19">
       <c r="A35" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B35" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C35" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D35" t="s">
         <v>22</v>
@@ -6082,7 +6076,7 @@
         <v>139</v>
       </c>
       <c r="P35" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="Q35">
         <v>0.45</v>
@@ -6096,13 +6090,13 @@
     </row>
     <row r="36" spans="1:19">
       <c r="A36" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B36" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C36" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D36" t="s">
         <v>30</v>
@@ -6141,7 +6135,7 @@
         <v>140</v>
       </c>
       <c r="P36" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="Q36">
         <v>0.17948700000000001</v>
@@ -6155,13 +6149,13 @@
     </row>
     <row r="37" spans="1:19">
       <c r="A37" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B37" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C37" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D37" t="s">
         <v>30</v>
@@ -6200,7 +6194,7 @@
         <v>141</v>
       </c>
       <c r="P37" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="Q37">
         <v>0.23255799999999999</v>
@@ -6214,13 +6208,13 @@
     </row>
     <row r="38" spans="1:19">
       <c r="A38" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B38" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C38" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D38" t="s">
         <v>26</v>
@@ -6259,7 +6253,7 @@
         <v>142</v>
       </c>
       <c r="P38" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="Q38">
         <v>0.252747</v>
@@ -6273,13 +6267,13 @@
     </row>
     <row r="39" spans="1:19">
       <c r="A39" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B39" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C39" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D39" t="s">
         <v>17</v>
@@ -6332,13 +6326,13 @@
     </row>
     <row r="40" spans="1:19">
       <c r="A40" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B40" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C40" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D40" t="s">
         <v>30</v>
@@ -6377,7 +6371,7 @@
         <v>140</v>
       </c>
       <c r="P40" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="Q40">
         <v>0.222222</v>
@@ -6391,13 +6385,13 @@
     </row>
     <row r="41" spans="1:19">
       <c r="A41" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B41" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C41" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D41" t="s">
         <v>18</v>
@@ -6436,7 +6430,7 @@
         <v>138</v>
       </c>
       <c r="P41" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="Q41">
         <v>0.2</v>
@@ -6450,13 +6444,13 @@
     </row>
     <row r="42" spans="1:19">
       <c r="A42" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B42" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C42" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D42" t="s">
         <v>30</v>
@@ -6495,7 +6489,7 @@
         <v>141</v>
       </c>
       <c r="P42" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="Q42">
         <v>0.15625</v>
@@ -6509,13 +6503,13 @@
     </row>
     <row r="43" spans="1:19">
       <c r="A43" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B43" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C43" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D43" t="s">
         <v>31</v>
@@ -6554,7 +6548,7 @@
         <v>143</v>
       </c>
       <c r="P43" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="Q43">
         <v>0.21276600000000001</v>
@@ -6568,13 +6562,13 @@
     </row>
     <row r="44" spans="1:19">
       <c r="A44" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B44" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C44" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D44" t="s">
         <v>31</v>
@@ -6613,7 +6607,7 @@
         <v>144</v>
       </c>
       <c r="P44" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="Q44">
         <v>0.26666699999999999</v>
@@ -6627,13 +6621,13 @@
     </row>
     <row r="45" spans="1:19">
       <c r="A45" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B45" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C45" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D45" t="s">
         <v>31</v>
@@ -6672,7 +6666,7 @@
         <v>143</v>
       </c>
       <c r="P45" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="Q45">
         <v>0.31547599999999998</v>
@@ -6686,13 +6680,13 @@
     </row>
     <row r="46" spans="1:19">
       <c r="A46" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B46" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C46" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D46" t="s">
         <v>31</v>
@@ -6731,7 +6725,7 @@
         <v>144</v>
       </c>
       <c r="P46" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="Q46">
         <v>0.286885</v>
@@ -6745,13 +6739,13 @@
     </row>
     <row r="47" spans="1:19">
       <c r="A47" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B47" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C47" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D47" t="s">
         <v>121</v>
@@ -6790,7 +6784,7 @@
         <v>145</v>
       </c>
       <c r="P47" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="Q47">
         <v>0.41836699999999999</v>
@@ -6804,13 +6798,13 @@
     </row>
     <row r="48" spans="1:19">
       <c r="A48" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B48" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C48" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D48" t="s">
         <v>27</v>
@@ -6849,7 +6843,7 @@
         <v>146</v>
       </c>
       <c r="P48" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="Q48">
         <v>0.15151500000000001</v>
@@ -6863,13 +6857,13 @@
     </row>
     <row r="49" spans="1:19">
       <c r="A49" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B49" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C49" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D49" t="s">
         <v>28</v>
@@ -6905,10 +6899,10 @@
         <v>45</v>
       </c>
       <c r="O49" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="P49" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="Q49">
         <v>0.57011500000000004</v>
@@ -6922,13 +6916,13 @@
     </row>
     <row r="50" spans="1:19">
       <c r="A50" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B50" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C50" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D50" t="s">
         <v>31</v>
@@ -6967,7 +6961,7 @@
         <v>147</v>
       </c>
       <c r="P50" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="Q50">
         <v>0.113043</v>
@@ -6981,13 +6975,13 @@
     </row>
     <row r="51" spans="1:19">
       <c r="A51" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B51" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C51" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D51" t="s">
         <v>22</v>
@@ -7026,7 +7020,7 @@
         <v>148</v>
       </c>
       <c r="P51" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="Q51">
         <v>0.22500000000000001</v>
@@ -7040,13 +7034,13 @@
     </row>
     <row r="52" spans="1:19">
       <c r="A52" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B52" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C52" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D52" t="s">
         <v>28</v>
@@ -7085,7 +7079,7 @@
         <v>149</v>
       </c>
       <c r="P52" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="Q52">
         <v>0.769231</v>
@@ -7099,13 +7093,13 @@
     </row>
     <row r="53" spans="1:19">
       <c r="A53" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B53" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C53" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D53" t="s">
         <v>18</v>
@@ -7144,7 +7138,7 @@
         <v>150</v>
       </c>
       <c r="P53" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="Q53">
         <v>0.125</v>
@@ -7158,13 +7152,13 @@
     </row>
     <row r="54" spans="1:19">
       <c r="A54" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B54" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C54" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D54" t="s">
         <v>22</v>
@@ -7203,7 +7197,7 @@
         <v>148</v>
       </c>
       <c r="P54" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="Q54">
         <v>0.38888899999999998</v>
@@ -7217,13 +7211,13 @@
     </row>
     <row r="55" spans="1:19">
       <c r="A55" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B55" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C55" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D55" t="s">
         <v>28</v>
@@ -7262,7 +7256,7 @@
         <v>149</v>
       </c>
       <c r="P55" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="Q55">
         <v>0.82857099999999995</v>
@@ -7276,13 +7270,13 @@
     </row>
     <row r="56" spans="1:19">
       <c r="A56" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B56" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="C56" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D56" t="s">
         <v>28</v>
@@ -7318,10 +7312,10 @@
         <v>45</v>
       </c>
       <c r="O56" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="P56" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="Q56">
         <v>0.605263</v>
@@ -7335,13 +7329,13 @@
     </row>
     <row r="57" spans="1:19">
       <c r="A57" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B57" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="C57" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D57" t="s">
         <v>22</v>
@@ -7380,7 +7374,7 @@
         <v>151</v>
       </c>
       <c r="P57" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="Q57">
         <v>0.28571400000000002</v>
@@ -7394,13 +7388,13 @@
     </row>
     <row r="58" spans="1:19">
       <c r="A58" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B58" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="C58" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D58" t="s">
         <v>32</v>
@@ -7439,7 +7433,7 @@
         <v>152</v>
       </c>
       <c r="P58" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="Q58">
         <v>0.28000000000000003</v>
@@ -7453,13 +7447,13 @@
     </row>
     <row r="59" spans="1:19">
       <c r="A59" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B59" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="C59" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D59" t="s">
         <v>17</v>
@@ -7512,13 +7506,13 @@
     </row>
     <row r="60" spans="1:19">
       <c r="A60" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B60" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="C60" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D60" t="s">
         <v>28</v>
@@ -7554,10 +7548,10 @@
         <v>45</v>
       </c>
       <c r="O60" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="P60" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="Q60">
         <v>0.32</v>
@@ -7571,13 +7565,13 @@
     </row>
     <row r="61" spans="1:19">
       <c r="A61" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B61" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C61" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D61" t="s">
         <v>19</v>
@@ -7616,7 +7610,7 @@
         <v>153</v>
       </c>
       <c r="P61" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Q61">
         <v>0.67045500000000002</v>
@@ -7630,13 +7624,13 @@
     </row>
     <row r="62" spans="1:19">
       <c r="A62" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B62" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C62" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D62" t="s">
         <v>17</v>
@@ -7689,13 +7683,13 @@
     </row>
     <row r="63" spans="1:19">
       <c r="A63" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B63" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C63" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D63" t="s">
         <v>24</v>
@@ -7734,7 +7728,7 @@
         <v>154</v>
       </c>
       <c r="P63" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="Q63">
         <v>0.14427899999999999</v>
@@ -7748,13 +7742,13 @@
     </row>
     <row r="64" spans="1:19">
       <c r="A64" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B64" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C64" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D64" t="s">
         <v>29</v>
@@ -7801,13 +7795,13 @@
     </row>
     <row r="65" spans="1:19">
       <c r="A65" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B65" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C65" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D65" t="s">
         <v>21</v>
@@ -7854,13 +7848,13 @@
     </row>
     <row r="66" spans="1:19">
       <c r="A66" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B66" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C66" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D66" t="s">
         <v>123</v>
@@ -7896,10 +7890,10 @@
         <v>45</v>
       </c>
       <c r="O66" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="P66" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="Q66">
         <v>0.48471599999999998</v>
@@ -7913,13 +7907,13 @@
     </row>
     <row r="67" spans="1:19">
       <c r="A67" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B67" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C67" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D67" t="s">
         <v>21</v>
@@ -7958,7 +7952,7 @@
         <v>155</v>
       </c>
       <c r="P67" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="Q67">
         <v>0.26506000000000002</v>
@@ -7972,13 +7966,13 @@
     </row>
     <row r="68" spans="1:19">
       <c r="A68" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B68" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C68" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D68" t="s">
         <v>21</v>
@@ -8017,7 +8011,7 @@
         <v>156</v>
       </c>
       <c r="P68" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="Q68">
         <v>0.264706</v>
@@ -8031,13 +8025,13 @@
     </row>
     <row r="69" spans="1:19">
       <c r="A69" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B69" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C69" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D69" t="s">
         <v>32</v>
@@ -8076,7 +8070,7 @@
         <v>157</v>
       </c>
       <c r="P69" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="Q69">
         <v>0.30232599999999998</v>
@@ -8090,13 +8084,13 @@
     </row>
     <row r="70" spans="1:19">
       <c r="A70" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B70" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C70" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D70" t="s">
         <v>21</v>
@@ -8135,7 +8129,7 @@
         <v>158</v>
       </c>
       <c r="P70" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="Q70">
         <v>9.2592999999999995E-2</v>
@@ -8149,13 +8143,13 @@
     </row>
     <row r="71" spans="1:19">
       <c r="A71" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B71" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C71" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D71" t="s">
         <v>17</v>
@@ -8208,13 +8202,13 @@
     </row>
     <row r="72" spans="1:19">
       <c r="A72" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B72" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C72" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D72" t="s">
         <v>121</v>
@@ -8253,7 +8247,7 @@
         <v>159</v>
       </c>
       <c r="P72" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="Q72">
         <v>0.96</v>
@@ -8267,13 +8261,13 @@
     </row>
     <row r="73" spans="1:19">
       <c r="A73" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B73" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C73" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D73" t="s">
         <v>21</v>
@@ -8312,7 +8306,7 @@
         <v>160</v>
       </c>
       <c r="P73" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="Q73">
         <v>0.227273</v>
@@ -8325,232 +8319,175 @@
       </c>
     </row>
     <row r="74" spans="1:19">
-      <c r="A74" t="s">
-        <v>251</v>
-      </c>
-      <c r="B74" t="s">
-        <v>308</v>
-      </c>
-      <c r="C74" t="s">
-        <v>270</v>
-      </c>
-      <c r="D74" t="s">
-        <v>25</v>
-      </c>
-      <c r="E74">
-        <v>2475</v>
-      </c>
-      <c r="F74">
-        <v>37</v>
-      </c>
-      <c r="G74">
-        <v>1</v>
-      </c>
-      <c r="H74">
-        <v>11168265</v>
-      </c>
-      <c r="I74">
-        <v>11168265</v>
-      </c>
-      <c r="J74" t="s">
-        <v>37</v>
-      </c>
-      <c r="K74" t="s">
-        <v>40</v>
-      </c>
-      <c r="L74" t="s">
+      <c r="A74" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E74" s="1">
+        <v>0</v>
+      </c>
+      <c r="F74" s="1">
+        <v>37</v>
+      </c>
+      <c r="G74" s="1">
+        <v>4</v>
+      </c>
+      <c r="H74" s="1">
+        <v>153245513</v>
+      </c>
+      <c r="I74" s="1">
+        <v>153245513</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L74" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M74" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N74" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O74" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="P74" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q74" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="R74" s="1">
+        <v>7</v>
+      </c>
+      <c r="S74" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19">
+      <c r="A75" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="1">
+        <v>58508</v>
+      </c>
+      <c r="F75" s="1">
+        <v>37</v>
+      </c>
+      <c r="G75" s="1">
+        <v>7</v>
+      </c>
+      <c r="H75" s="1">
+        <v>152007050</v>
+      </c>
+      <c r="I75" s="1">
+        <v>152007050</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L75" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M75" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="M74" t="s">
+      <c r="N75" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O75" s="1"/>
+      <c r="P75" s="1"/>
+      <c r="Q75" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="R75" s="1">
+        <v>13</v>
+      </c>
+      <c r="S75" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19">
+      <c r="A76" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E76" s="1">
+        <v>0</v>
+      </c>
+      <c r="F76" s="1">
+        <v>37</v>
+      </c>
+      <c r="G76" s="1">
+        <v>4</v>
+      </c>
+      <c r="H76" s="1">
+        <v>153245518</v>
+      </c>
+      <c r="I76" s="1">
+        <v>153245518</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L76" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N74" t="s">
-        <v>45</v>
-      </c>
-      <c r="O74" t="s">
-        <v>137</v>
-      </c>
-      <c r="P74" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q74">
-        <v>8.1081E-2</v>
-      </c>
-      <c r="R74">
+      <c r="M76" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N76" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O76" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="P76" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q76" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="R76" s="1">
         <v>9</v>
       </c>
-      <c r="S74">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="75" spans="1:19">
-      <c r="A75" t="s">
-        <v>252</v>
-      </c>
-      <c r="B75" t="s">
-        <v>309</v>
-      </c>
-      <c r="C75" t="s">
-        <v>270</v>
-      </c>
-      <c r="D75" t="s">
-        <v>30</v>
-      </c>
-      <c r="E75">
-        <v>0</v>
-      </c>
-      <c r="F75">
-        <v>37</v>
-      </c>
-      <c r="G75">
-        <v>4</v>
-      </c>
-      <c r="H75">
-        <v>153245513</v>
-      </c>
-      <c r="I75">
-        <v>153245513</v>
-      </c>
-      <c r="J75" t="s">
-        <v>37</v>
-      </c>
-      <c r="K75" t="s">
-        <v>40</v>
-      </c>
-      <c r="L75" t="s">
-        <v>42</v>
-      </c>
-      <c r="M75" t="s">
-        <v>41</v>
-      </c>
-      <c r="N75" t="s">
-        <v>45</v>
-      </c>
-      <c r="O75" t="s">
-        <v>161</v>
-      </c>
-      <c r="P75" t="s">
-        <v>206</v>
-      </c>
-      <c r="Q75">
-        <v>0.35</v>
-      </c>
-      <c r="R75">
-        <v>7</v>
-      </c>
-      <c r="S75">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="76" spans="1:19">
-      <c r="A76" t="s">
-        <v>252</v>
-      </c>
-      <c r="B76" t="s">
-        <v>309</v>
-      </c>
-      <c r="C76" t="s">
-        <v>270</v>
-      </c>
-      <c r="D76" t="s">
-        <v>21</v>
-      </c>
-      <c r="E76">
-        <v>58508</v>
-      </c>
-      <c r="F76">
-        <v>37</v>
-      </c>
-      <c r="G76">
-        <v>7</v>
-      </c>
-      <c r="H76">
-        <v>152007050</v>
-      </c>
-      <c r="I76">
-        <v>152007050</v>
-      </c>
-      <c r="J76" t="s">
-        <v>124</v>
-      </c>
-      <c r="K76" t="s">
-        <v>40</v>
-      </c>
-      <c r="L76" t="s">
-        <v>42</v>
-      </c>
-      <c r="M76" t="s">
-        <v>43</v>
-      </c>
-      <c r="N76" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q76">
-        <v>0.5</v>
-      </c>
-      <c r="R76">
-        <v>13</v>
-      </c>
-      <c r="S76">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="77" spans="1:19">
-      <c r="A77" t="s">
-        <v>252</v>
-      </c>
-      <c r="B77" t="s">
-        <v>309</v>
-      </c>
-      <c r="C77" t="s">
-        <v>270</v>
-      </c>
-      <c r="D77" t="s">
-        <v>30</v>
-      </c>
-      <c r="E77">
-        <v>0</v>
-      </c>
-      <c r="F77">
-        <v>37</v>
-      </c>
-      <c r="G77">
-        <v>4</v>
-      </c>
-      <c r="H77">
-        <v>153245518</v>
-      </c>
-      <c r="I77">
-        <v>153245518</v>
-      </c>
-      <c r="J77" t="s">
-        <v>37</v>
-      </c>
-      <c r="K77" t="s">
-        <v>40</v>
-      </c>
-      <c r="L77" t="s">
-        <v>41</v>
-      </c>
-      <c r="M77" t="s">
-        <v>44</v>
-      </c>
-      <c r="N77" t="s">
-        <v>45</v>
-      </c>
-      <c r="O77" t="s">
-        <v>162</v>
-      </c>
-      <c r="P77" t="s">
-        <v>207</v>
-      </c>
-      <c r="Q77">
-        <v>0.6</v>
-      </c>
-      <c r="R77">
-        <v>9</v>
-      </c>
-      <c r="S77">
+      <c r="S76" s="1">
         <v>6</v>
       </c>
     </row>

</xml_diff>